<commit_message>
Add monitor design. The host access can be transfer to the PC via the serial port.
git-svn-id: http://192.168.1.99/svn/lcdc@7 532a5362-acf3-9844-9c1a-8320e3097434
</commit_message>
<xml_diff>
--- a/epson/s1d13700/dev/hw/brd/pdf/s1d13700_bom.xlsx
+++ b/epson/s1d13700/dev/hw/brd/pdf/s1d13700_bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="92">
   <si>
     <t>HOST I/F  Revised: Thursday, August 09, 2012</t>
   </si>
@@ -255,10 +255,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>I/F</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Backlight</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -319,15 +315,35 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>胶体颜色？绿色</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>10V</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>绕线</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>电压/10V</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>绿色</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10MHz振荡器</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>主机接口-插针</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3V/5V I/F</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -483,18 +499,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -667,6 +677,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -790,6 +818,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -823,7 +854,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -841,9 +872,6 @@
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -859,19 +887,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -883,6 +911,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -898,40 +929,52 @@
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1268,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1282,603 +1325,612 @@
     <col min="6" max="7" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
-      <c r="A15">
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B15">
+      <c r="B10" s="2">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
+      <c r="F10" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1">
+      <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B16">
+      <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E11" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17">
+    <row r="12" spans="1:7" s="2" customFormat="1">
+      <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B17">
+      <c r="B12" s="2">
         <v>7</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A13" s="2">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2">
+        <v>27</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A14" s="2">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1206</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A15" s="2">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="2" customFormat="1">
+      <c r="A16" s="2">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="2" customFormat="1">
+      <c r="A17" s="2">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="3">
+        <v>33</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1">
       <c r="A18" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2">
-        <v>27</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1" ht="27">
       <c r="A19" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B19" s="2">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>48</v>
+        <v>16</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="4">
-        <v>1206</v>
+        <v>59</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="20" spans="1:8" s="2" customFormat="1">
       <c r="A20" s="2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1">
       <c r="A21" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B21" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="2" customFormat="1">
       <c r="A22" s="2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B22" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="4">
         <v>33</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>84</v>
+      <c r="D22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="2" customFormat="1">
       <c r="A23" s="2">
+        <v>14</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1">
+      <c r="A24" s="2">
+        <v>15</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="5" customFormat="1">
+      <c r="A26" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="5" customFormat="1">
+      <c r="A27" s="5">
+        <v>16</v>
+      </c>
+      <c r="B27" s="5">
+        <v>2</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="5" customFormat="1">
+      <c r="A28" s="5">
+        <v>17</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="5" customFormat="1" ht="15" customHeight="1">
+      <c r="A29" s="5">
+        <v>18</v>
+      </c>
+      <c r="B29" s="5">
+        <v>2</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="2">
+      <c r="E29" s="6">
+        <v>1206</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="5" customFormat="1" ht="15" customHeight="1">
+      <c r="A30" s="5">
+        <v>19</v>
+      </c>
+      <c r="B30" s="5">
+        <v>2</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="5" customFormat="1">
+      <c r="A31" s="5">
+        <v>20</v>
+      </c>
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" s="8" customFormat="1">
+      <c r="A33" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1">
+      <c r="A34" s="8">
+        <v>21</v>
+      </c>
+      <c r="B34" s="8">
+        <v>1</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="9">
+        <v>1210</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="8" customFormat="1">
+      <c r="A35" s="8">
+        <v>22</v>
+      </c>
+      <c r="B35" s="8">
+        <v>3</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1">
+      <c r="A36" s="8">
+        <v>23</v>
+      </c>
+      <c r="B36" s="8">
+        <v>2</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="D36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1">
+      <c r="A37" s="8">
+        <v>24</v>
+      </c>
+      <c r="B37" s="8">
+        <v>1</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="8" customFormat="1">
+      <c r="A38" s="8">
+        <v>25</v>
+      </c>
+      <c r="B38" s="8">
+        <v>1</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="8" customFormat="1">
+      <c r="A39" s="8">
+        <v>26</v>
+      </c>
+      <c r="B39" s="8">
+        <v>1</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" ht="27">
-      <c r="A24" s="2">
-        <v>10</v>
-      </c>
-      <c r="B24" s="2">
+      <c r="G39" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1">
+      <c r="A40" s="8">
+        <v>27</v>
+      </c>
+      <c r="B40" s="8">
+        <v>1</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1">
+      <c r="A41" s="8">
+        <v>28</v>
+      </c>
+      <c r="B41" s="8">
+        <v>1</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25">
-        <v>11</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26">
-        <v>12</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="2" customFormat="1">
-      <c r="A27" s="2">
-        <v>13</v>
-      </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="2" customFormat="1">
-      <c r="A28" s="2">
-        <v>14</v>
-      </c>
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="2" customFormat="1">
-      <c r="A29" s="2">
-        <v>15</v>
-      </c>
-      <c r="B29" s="2">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="2" customFormat="1">
-      <c r="A32" s="2">
-        <v>16</v>
-      </c>
-      <c r="B32" s="2">
-        <v>2</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="2" customFormat="1">
-      <c r="A33" s="2">
+      <c r="D41" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="2">
-        <v>1</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A34" s="2">
-        <v>18</v>
-      </c>
-      <c r="B34" s="2">
-        <v>2</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="4">
-        <v>1206</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A35" s="2">
-        <v>19</v>
-      </c>
-      <c r="B35" s="2">
-        <v>2</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="2" customFormat="1">
-      <c r="A36" s="2">
-        <v>20</v>
-      </c>
-      <c r="B36" s="2">
-        <v>1</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="4">
-        <v>0</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="2">
-        <v>21</v>
-      </c>
-      <c r="B39" s="2">
-        <v>1</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" s="4">
-        <v>1210</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="2" customFormat="1">
-      <c r="A40" s="2">
-        <v>22</v>
-      </c>
-      <c r="B40" s="2">
-        <v>3</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D40" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A41" s="2">
-        <v>23</v>
-      </c>
-      <c r="B41" s="2">
-        <v>2</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A42" s="2">
-        <v>24</v>
-      </c>
-      <c r="B42" s="2">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" s="2" customFormat="1">
-      <c r="A43" s="2">
-        <v>25</v>
-      </c>
-      <c r="B43" s="2">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="2" customFormat="1">
-      <c r="A44" s="2">
-        <v>26</v>
-      </c>
-      <c r="B44" s="2">
-        <v>1</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1">
-      <c r="A45" s="5">
-        <v>27</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" s="1" t="s">
+      <c r="E41" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F45" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1">
-      <c r="A46" s="5">
-        <v>28</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="F41" s="8" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>